<commit_message>
Add Previous Java Prototype
- Promoted Elements Model
- Change Elements .xlsx a bit
</commit_message>
<xml_diff>
--- a/研发文档/Elements.xlsx
+++ b/研发文档/Elements.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BLACSTAR\Documents\GitHub\MonsterTrainer\研发文档\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24795" windowHeight="15615" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24780" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Restriction" sheetId="1" r:id="rId1"/>
@@ -91,11 +86,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -111,7 +106,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -120,7 +115,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -130,6 +125,14 @@
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -278,7 +281,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -311,87 +314,90 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="79">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -731,12 +737,12 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="10.875" style="1"/>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -799,7 +805,7 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="12">
         <v>1</v>
       </c>
       <c r="C2" s="9">
@@ -854,7 +860,7 @@
       <c r="B3" s="9">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="12">
         <v>1</v>
       </c>
       <c r="D3" s="9">
@@ -909,7 +915,7 @@
       <c r="C4" s="9">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="12">
         <v>1</v>
       </c>
       <c r="E4" s="9">
@@ -964,7 +970,7 @@
       <c r="D5" s="9">
         <v>1.1499999999999999</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="12">
         <v>1</v>
       </c>
       <c r="F5" s="9">
@@ -1019,7 +1025,7 @@
       <c r="E6" s="9">
         <v>0.7</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="12">
         <v>1</v>
       </c>
       <c r="G6" s="9">
@@ -1074,7 +1080,7 @@
       <c r="F7" s="9">
         <v>1.1499999999999999</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="12">
         <v>1</v>
       </c>
       <c r="H7" s="9">
@@ -1129,7 +1135,7 @@
       <c r="G8" s="9">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="12">
         <v>1</v>
       </c>
       <c r="I8" s="9">
@@ -1184,7 +1190,7 @@
       <c r="H9" s="9">
         <v>1.1499999999999999</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="12">
         <v>1</v>
       </c>
       <c r="J9" s="9">
@@ -1239,7 +1245,7 @@
       <c r="I10" s="9">
         <v>1</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="12">
         <v>1</v>
       </c>
       <c r="K10" s="9">
@@ -1294,7 +1300,7 @@
       <c r="J11" s="9">
         <v>1.1499999999999999</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="12">
         <v>1</v>
       </c>
       <c r="L11" s="9">
@@ -1349,7 +1355,7 @@
       <c r="K12" s="9">
         <v>1</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="12">
         <v>1</v>
       </c>
       <c r="M12" s="9">
@@ -1404,7 +1410,7 @@
       <c r="L13" s="9">
         <v>1.1499999999999999</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="12">
         <v>1</v>
       </c>
       <c r="N13" s="9">
@@ -1459,7 +1465,7 @@
       <c r="M14" s="9">
         <v>1.1499999999999999</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="12">
         <v>1</v>
       </c>
       <c r="O14" s="9">
@@ -1514,7 +1520,7 @@
       <c r="N15" s="9">
         <v>1.1499999999999999</v>
       </c>
-      <c r="O15" s="9">
+      <c r="O15" s="12">
         <v>1</v>
       </c>
       <c r="P15" s="9">
@@ -1569,7 +1575,7 @@
       <c r="O16" s="9">
         <v>1.1499999999999999</v>
       </c>
-      <c r="P16" s="9">
+      <c r="P16" s="12">
         <v>1</v>
       </c>
       <c r="Q16" s="9"/>
@@ -1594,7 +1600,7 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
-      <c r="Q17" s="9">
+      <c r="Q17" s="12">
         <v>1</v>
       </c>
       <c r="R17" s="9"/>
@@ -1619,7 +1625,7 @@
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
-      <c r="R18" s="9">
+      <c r="R18" s="12">
         <v>1</v>
       </c>
     </row>
@@ -1639,10 +1645,10 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="11" t="s">

</xml_diff>

<commit_message>
Update Models & Elements
Add PP
</commit_message>
<xml_diff>
--- a/研发文档/Elements.xlsx
+++ b/研发文档/Elements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24800" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Restriction" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
   <si>
     <t>攻击\防御</t>
   </si>
@@ -79,9 +79,6 @@
     <t>融合</t>
   </si>
   <si>
-    <t>芽 Growth</t>
-  </si>
-  <si>
     <t>光 Light</t>
   </si>
   <si>
@@ -92,6 +89,12 @@
   </si>
   <si>
     <t>时 Time</t>
+  </si>
+  <si>
+    <t>树 Plant</t>
+  </si>
+  <si>
+    <t>木 Wood</t>
   </si>
 </sst>
 </file>
@@ -212,8 +215,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -339,7 +386,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -382,6 +429,28 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -424,6 +493,28 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -761,16 +852,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="16" width="10.83203125" style="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -780,29 +872,29 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>13</v>
@@ -817,7 +909,7 @@
         <v>2</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="P1" s="7" t="s">
         <v>16</v>
@@ -831,29 +923,29 @@
         <v>1</v>
       </c>
       <c r="C2" s="13">
-        <v>0.85</v>
+        <v>1.3</v>
       </c>
       <c r="D2" s="13">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="E2" s="13">
-        <v>1.1499999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="F2" s="13">
-        <v>1</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G2" s="13">
         <v>0.85</v>
       </c>
       <c r="H2" s="13">
-        <v>0.7</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="I2" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="J2" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J2" s="13">
-        <v>1.1499999999999999</v>
-      </c>
       <c r="K2" s="13">
         <v>1</v>
       </c>
@@ -874,394 +966,394 @@
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H3" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I3" s="13">
+        <v>1</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="K3" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L3" s="13">
+        <v>1</v>
+      </c>
+      <c r="M3" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="N3" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="O3" s="13">
+        <v>1</v>
+      </c>
+      <c r="P3" s="13">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="I4" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="J4" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L4" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="M4" s="13">
+        <v>1</v>
+      </c>
+      <c r="N4" s="13">
+        <v>1</v>
+      </c>
+      <c r="O4" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="P4" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H5" s="13">
+        <v>1</v>
+      </c>
+      <c r="I5" s="13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J5" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="K5" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="L5" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="M5" s="13">
+        <v>1</v>
+      </c>
+      <c r="N5" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="O5" s="13">
+        <v>1</v>
+      </c>
+      <c r="P5" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="13">
+        <v>1</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F6" s="12">
+        <v>1</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I6" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J6" s="13">
+        <v>1</v>
+      </c>
+      <c r="K6" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="L6" s="13">
+        <v>1</v>
+      </c>
+      <c r="M6" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="N6" s="13">
+        <v>1</v>
+      </c>
+      <c r="O6" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="P6" s="13">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="C3" s="12">
-        <v>1</v>
-      </c>
-      <c r="D3" s="13">
+      <c r="B7" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C7" s="13">
         <v>1.45</v>
       </c>
-      <c r="E3" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="F3" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="G3" s="13">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="I3" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="J3" s="13">
-        <v>1.3</v>
-      </c>
-      <c r="K3" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L3" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="M3" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="N3" s="13">
-        <v>1</v>
-      </c>
-      <c r="O3" s="13">
-        <v>1.3</v>
-      </c>
-      <c r="P3" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="C4" s="13">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="F4" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="G4" s="13">
-        <v>1</v>
-      </c>
-      <c r="H4" s="13">
-        <v>1</v>
-      </c>
-      <c r="I4" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="J4" s="13">
-        <v>1.3</v>
-      </c>
-      <c r="K4" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L4" s="13">
-        <v>1</v>
-      </c>
-      <c r="M4" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="N4" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="O4" s="13">
-        <v>1</v>
-      </c>
-      <c r="P4" s="13">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="C5" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="D5" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E5" s="12">
-        <v>1</v>
-      </c>
-      <c r="F5" s="13">
-        <v>1.3</v>
-      </c>
-      <c r="G5" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="H5" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="I5" s="13">
-        <v>1</v>
-      </c>
-      <c r="J5" s="13">
+      <c r="D7" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="G7" s="12">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I7" s="13">
+        <v>1</v>
+      </c>
+      <c r="J7" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="K7" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L7" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="M7" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="N7" s="13">
+        <v>1</v>
+      </c>
+      <c r="O7" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="P7" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F8" s="13">
         <v>1.45</v>
       </c>
-      <c r="K5" s="13">
-        <v>1.3</v>
-      </c>
-      <c r="L5" s="13">
-        <v>1.3</v>
-      </c>
-      <c r="M5" s="13">
-        <v>1</v>
-      </c>
-      <c r="N5" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="O5" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="P5" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="C6" s="13">
-        <v>1</v>
-      </c>
-      <c r="D6" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="E6" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="F6" s="12">
-        <v>1</v>
-      </c>
-      <c r="G6" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="H6" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="I6" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="J6" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="K6" s="13">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L6" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="M6" s="13">
-        <v>1</v>
-      </c>
-      <c r="N6" s="13">
-        <v>1</v>
-      </c>
-      <c r="O6" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="P6" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="6" t="s">
+      <c r="G8" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="H8" s="12">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="L8" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="M8" s="13">
+        <v>1</v>
+      </c>
+      <c r="N8" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="O8" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="P8" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="C7" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="D7" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E7" s="13">
-        <v>1</v>
-      </c>
-      <c r="F7" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="G7" s="12">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13">
+      <c r="B9" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C9" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E9" s="13">
         <v>1.45</v>
       </c>
-      <c r="I7" s="13">
-        <v>1.3</v>
-      </c>
-      <c r="J7" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="K7" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="L7" s="13">
-        <v>1</v>
-      </c>
-      <c r="M7" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="N7" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="O7" s="13">
-        <v>1</v>
-      </c>
-      <c r="P7" s="13">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="13">
-        <v>1.3</v>
-      </c>
-      <c r="C8" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="D8" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E8" s="13">
-        <v>1</v>
-      </c>
-      <c r="F8" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="G8" s="13">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="H8" s="12">
-        <v>1</v>
-      </c>
-      <c r="I8" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="J8" s="13">
-        <v>1</v>
-      </c>
-      <c r="K8" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="L8" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="M8" s="13">
-        <v>1</v>
-      </c>
-      <c r="N8" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="O8" s="13">
-        <v>1</v>
-      </c>
-      <c r="P8" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="4" t="s">
+      <c r="F9" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="G9" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H9" s="13">
+        <v>1</v>
+      </c>
+      <c r="I9" s="12">
+        <v>1</v>
+      </c>
+      <c r="J9" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="K9" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="L9" s="13">
+        <v>1</v>
+      </c>
+      <c r="M9" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="N9" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="O9" s="13">
+        <v>1</v>
+      </c>
+      <c r="P9" s="13">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B10" s="13">
         <v>1.45</v>
       </c>
-      <c r="C9" s="13">
-        <v>1.3</v>
-      </c>
-      <c r="D9" s="13">
-        <v>1.3</v>
-      </c>
-      <c r="E9" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="F9" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="G9" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="H9" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="I9" s="12">
-        <v>1</v>
-      </c>
-      <c r="J9" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="K9" s="13">
-        <v>1</v>
-      </c>
-      <c r="L9" s="13">
-        <v>1</v>
-      </c>
-      <c r="M9" s="13">
-        <v>1.3</v>
-      </c>
-      <c r="N9" s="13">
-        <v>1</v>
-      </c>
-      <c r="O9" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="P9" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="13">
-        <v>1</v>
-      </c>
       <c r="C10" s="13">
-        <v>0.7</v>
+        <v>1.3</v>
       </c>
       <c r="D10" s="13">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="E10" s="13">
-        <v>0.55000000000000004</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="F10" s="13">
-        <v>1.3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G10" s="13">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="H10" s="13">
         <v>1.1499999999999999</v>
       </c>
       <c r="I10" s="13">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="J10" s="12">
         <v>1</v>
       </c>
       <c r="K10" s="13">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="L10" s="13">
         <v>1</v>
       </c>
       <c r="M10" s="13">
-        <v>0.7</v>
+        <v>1.3</v>
       </c>
       <c r="N10" s="13">
         <v>1</v>
@@ -1270,7 +1362,7 @@
         <v>0.85</v>
       </c>
       <c r="P10" s="13">
-        <v>0.85</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1281,25 +1373,25 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="C11" s="13">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="D11" s="13">
-        <v>0.85</v>
+        <v>1.45</v>
       </c>
       <c r="E11" s="13">
-        <v>0.7</v>
+        <v>1.3</v>
       </c>
       <c r="F11" s="13">
-        <v>1.45</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G11" s="13">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="H11" s="13">
-        <v>1.3</v>
+        <v>0.7</v>
       </c>
       <c r="I11" s="13">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="J11" s="13">
         <v>1.1499999999999999</v>
@@ -1331,28 +1423,28 @@
         <v>1.45</v>
       </c>
       <c r="C12" s="13">
-        <v>1.3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="D12" s="13">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="E12" s="13">
-        <v>0.85</v>
+        <v>1.3</v>
       </c>
       <c r="F12" s="13">
-        <v>1.3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G12" s="13">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="H12" s="13">
-        <v>1.3</v>
+        <v>0.85</v>
       </c>
       <c r="I12" s="13">
         <v>1</v>
       </c>
       <c r="J12" s="13">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="K12" s="13">
         <v>1</v>
@@ -1381,28 +1473,28 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="C13" s="13">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="D13" s="13">
-        <v>1.3</v>
+        <v>1.45</v>
       </c>
       <c r="E13" s="13">
-        <v>1</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>1.45</v>
+        <v>1.3</v>
       </c>
       <c r="G13" s="13">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="H13" s="13">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="I13" s="13">
-        <v>0.85</v>
+        <v>1.3</v>
       </c>
       <c r="J13" s="13">
-        <v>1.3</v>
+        <v>0.85</v>
       </c>
       <c r="K13" s="13">
         <v>1.1499999999999999</v>
@@ -1431,28 +1523,28 @@
         <v>1.3</v>
       </c>
       <c r="C14" s="13">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="D14" s="13">
-        <v>1.3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="E14" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="F14" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G14" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H14" s="13">
         <v>1.45</v>
       </c>
-      <c r="F14" s="13">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="G14" s="13">
-        <v>1</v>
-      </c>
-      <c r="H14" s="13">
-        <v>1.3</v>
-      </c>
       <c r="I14" s="13">
         <v>1</v>
       </c>
       <c r="J14" s="13">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="K14" s="13">
         <v>0.85</v>
@@ -1475,31 +1567,31 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B15" s="13">
         <v>1.1499999999999999</v>
       </c>
       <c r="C15" s="13">
-        <v>0.85</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="D15" s="13">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="E15" s="13">
-        <v>1</v>
+        <v>1.45</v>
       </c>
       <c r="F15" s="13">
         <v>1.3</v>
       </c>
       <c r="G15" s="13">
-        <v>1.1499999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="H15" s="13">
-        <v>1.45</v>
+        <v>1</v>
       </c>
       <c r="I15" s="13">
-        <v>1.3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="J15" s="13">
         <v>1.3</v>
@@ -1531,28 +1623,28 @@
         <v>1.3</v>
       </c>
       <c r="C16" s="13">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="D16" s="13">
-        <v>1.3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="E16" s="13">
         <v>1.1499999999999999</v>
       </c>
       <c r="F16" s="13">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="G16" s="13">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="H16" s="13">
         <v>1.1499999999999999</v>
       </c>
       <c r="I16" s="13">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="J16" s="13">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="K16" s="13">
         <v>1.3</v>
@@ -1575,7 +1667,7 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1595,7 +1687,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1620,12 +1712,12 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>